<commit_message>
54 cerp and pbc monthly reports (#55)
* Update CERP_PBC_WQ_Summary_Data.xlsx

pH summary data corrections

* Update survey logic to run only in March and September

Changed conditional checks for survey-related code to execute only when Month is '03' or '09'

* Add monthly report templates for CERP and PBC

Added new RMarkdown files for generating CERP and PBC monthly reports from network files.
Archived the previous PBC Monthly Reports template.
</commit_message>
<xml_diff>
--- a/Data/CERP_PBC_WQ_Summary_Data.xlsx
+++ b/Data/CERP_PBC_WQ_Summary_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erica.Williams\Documents\GitHub\Oyster-Reports\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1237000-8413-4F55-A3DC-BD146807B74C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A75B6B5-79CB-4BB7-90BB-D7A4C989FF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DO Station" sheetId="1" r:id="rId1"/>
@@ -1541,7 +1541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1577,6 +1577,7 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -26372,7 +26373,7 @@
   <dimension ref="A1:AH28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A27" sqref="A27:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29093,7 +29094,7 @@
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="13">
         <v>45791</v>
       </c>
       <c r="B27">
@@ -29102,10 +29103,13 @@
       <c r="C27">
         <v>8.2799999999999994</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="13">
         <v>45791</v>
       </c>
-      <c r="G27" s="9">
+      <c r="E27">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="G27" s="13">
         <v>45783</v>
       </c>
       <c r="H27">
@@ -29117,7 +29121,7 @@
       <c r="J27">
         <v>8.17</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="13">
         <v>45783</v>
       </c>
       <c r="L27">
@@ -29129,7 +29133,7 @@
       <c r="N27">
         <v>8.31</v>
       </c>
-      <c r="O27" s="9">
+      <c r="O27" s="13">
         <v>45783</v>
       </c>
       <c r="P27">
@@ -29141,7 +29145,7 @@
       <c r="R27">
         <v>8.3000000000000007</v>
       </c>
-      <c r="S27" s="9">
+      <c r="S27" s="13">
         <v>45783</v>
       </c>
       <c r="T27">
@@ -29153,7 +29157,7 @@
       <c r="V27">
         <v>8.25</v>
       </c>
-      <c r="W27" s="9">
+      <c r="W27" s="13">
         <v>45784</v>
       </c>
       <c r="X27">
@@ -29165,7 +29169,7 @@
       <c r="Z27">
         <v>7.88</v>
       </c>
-      <c r="AA27" s="9">
+      <c r="AA27" s="13">
         <v>45784</v>
       </c>
       <c r="AB27">
@@ -29177,7 +29181,7 @@
       <c r="AD27">
         <v>7.85</v>
       </c>
-      <c r="AE27" s="9">
+      <c r="AE27" s="13">
         <v>45784</v>
       </c>
       <c r="AF27">
@@ -29191,13 +29195,13 @@
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="13">
         <v>45825</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="13">
         <v>45825</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="13">
         <v>45818</v>
       </c>
       <c r="H28">
@@ -29209,7 +29213,7 @@
       <c r="J28">
         <v>8.39</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="13">
         <v>45818</v>
       </c>
       <c r="L28">
@@ -29221,7 +29225,7 @@
       <c r="N28">
         <v>8.89</v>
       </c>
-      <c r="O28" s="2">
+      <c r="O28" s="13">
         <v>45818</v>
       </c>
       <c r="P28">
@@ -29233,7 +29237,7 @@
       <c r="R28">
         <v>8.0399999999999991</v>
       </c>
-      <c r="S28" s="2">
+      <c r="S28" s="13">
         <v>45818</v>
       </c>
       <c r="T28">
@@ -29245,7 +29249,7 @@
       <c r="V28">
         <v>8.18</v>
       </c>
-      <c r="W28" s="2">
+      <c r="W28" s="13">
         <v>45819</v>
       </c>
       <c r="X28">
@@ -29257,7 +29261,7 @@
       <c r="Z28">
         <v>7.89</v>
       </c>
-      <c r="AA28" s="2">
+      <c r="AA28" s="13">
         <v>45819</v>
       </c>
       <c r="AB28">
@@ -29269,7 +29273,7 @@
       <c r="AD28">
         <v>8.18</v>
       </c>
-      <c r="AE28" s="2">
+      <c r="AE28" s="13">
         <v>45819</v>
       </c>
       <c r="AF28">
@@ -29292,8 +29296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AS28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32872,7 +32876,7 @@
       </c>
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="13">
         <v>45791</v>
       </c>
       <c r="B27">
@@ -32887,10 +32891,19 @@
       <c r="E27">
         <v>8.2799999999999994</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="13">
         <v>45791</v>
       </c>
-      <c r="K27" s="9">
+      <c r="G27">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="I27">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="J27">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="K27" s="13">
         <v>45783</v>
       </c>
       <c r="L27">
@@ -32905,7 +32918,7 @@
       <c r="O27">
         <v>8.32</v>
       </c>
-      <c r="P27" s="9">
+      <c r="P27" s="13">
         <v>45783</v>
       </c>
       <c r="Q27">
@@ -32920,7 +32933,7 @@
       <c r="T27">
         <v>8.31</v>
       </c>
-      <c r="U27" s="9">
+      <c r="U27" s="13">
         <v>45783</v>
       </c>
       <c r="V27">
@@ -32935,7 +32948,7 @@
       <c r="Y27">
         <v>8.31</v>
       </c>
-      <c r="Z27" s="9">
+      <c r="Z27" s="13">
         <v>45783</v>
       </c>
       <c r="AA27">
@@ -32950,7 +32963,7 @@
       <c r="AD27">
         <v>8.2899999999999991</v>
       </c>
-      <c r="AE27" s="9">
+      <c r="AE27" s="13">
         <v>45784</v>
       </c>
       <c r="AF27">
@@ -32965,7 +32978,7 @@
       <c r="AI27">
         <v>7.88</v>
       </c>
-      <c r="AJ27" s="9">
+      <c r="AJ27" s="13">
         <v>45784</v>
       </c>
       <c r="AK27">
@@ -32980,7 +32993,7 @@
       <c r="AN27">
         <v>7.99</v>
       </c>
-      <c r="AO27" s="9">
+      <c r="AO27" s="13">
         <v>45784</v>
       </c>
       <c r="AP27">
@@ -32997,13 +33010,13 @@
       </c>
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="13">
         <v>45825</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="13">
         <v>45825</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="13">
         <v>45818</v>
       </c>
       <c r="L28">
@@ -33018,7 +33031,7 @@
       <c r="O28">
         <v>8.56</v>
       </c>
-      <c r="P28" s="2">
+      <c r="P28" s="13">
         <v>45818</v>
       </c>
       <c r="Q28">
@@ -33033,7 +33046,7 @@
       <c r="T28">
         <v>8.89</v>
       </c>
-      <c r="U28" s="2">
+      <c r="U28" s="13">
         <v>45818</v>
       </c>
       <c r="V28">
@@ -33048,7 +33061,7 @@
       <c r="Y28">
         <v>8.09</v>
       </c>
-      <c r="Z28" s="2">
+      <c r="Z28" s="13">
         <v>45818</v>
       </c>
       <c r="AA28">
@@ -33063,7 +33076,7 @@
       <c r="AD28">
         <v>8.31</v>
       </c>
-      <c r="AE28" s="2">
+      <c r="AE28" s="13">
         <v>45819</v>
       </c>
       <c r="AF28">
@@ -33078,7 +33091,7 @@
       <c r="AI28">
         <v>8.02</v>
       </c>
-      <c r="AJ28" s="2">
+      <c r="AJ28" s="13">
         <v>45819</v>
       </c>
       <c r="AK28">
@@ -33093,7 +33106,7 @@
       <c r="AN28">
         <v>8.18</v>
       </c>
-      <c r="AO28" s="2">
+      <c r="AO28" s="13">
         <v>45819</v>
       </c>
       <c r="AP28">
@@ -33119,7 +33132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AH28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>